<commit_message>
update sin tildes ni index en las tablas
</commit_message>
<xml_diff>
--- a/InformeFICs.xlsx
+++ b/InformeFICs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bancolombia-my.sharepoint.com/personal/juliavar_bancolombia_com_co/Documents/Workspace/PruebaStreamLit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{5DDB5F60-F557-43A4-AC66-48309A183593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E922E15C-4FF5-447B-BA20-84F634BBFE1F}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{5DDB5F60-F557-43A4-AC66-48309A183593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AF4FA6A-1020-4D0B-815B-99ABF56DFA8D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F3D96AE9-0F86-4742-BBBC-4A4B76F80A99}"/>
   </bookViews>
@@ -57,13 +57,7 @@
     <t>BBVA FIDUCIARIA S.A.</t>
   </si>
   <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO BBVA PAÍS CON PARTICIPACIONES DIFERENCIALES</t>
-  </si>
-  <si>
     <t>CREDICORP CAPITAL FIDUCIARIA S.A.</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO FIDUCREDICORP VISTA</t>
   </si>
   <si>
     <t>FIDUAGRARIA S.A.</t>
@@ -79,9 +73,6 @@
   </si>
   <si>
     <t>FIDUCIARIA BANCOLOMBIA S.A.</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTA SIN PACTO DE PERMANENCIA FIDUEXCEDENTES</t>
   </si>
   <si>
     <t>FIDUCIARIA BOGOTA S.A.</t>
@@ -111,22 +102,10 @@
     <t>FIDUCIARIA POPULAR S.A.</t>
   </si>
   <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO FIDULIQUIDEZ</t>
-  </si>
-  <si>
     <t>FIDUCOLDEX S.A.</t>
   </si>
   <si>
-    <t xml:space="preserve">FONDO DE INVERSIÓN COLECTIVA FIDUCOLDEX </t>
-  </si>
-  <si>
     <t>FIDUOCCIDENTE S.A.</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO SIN PACTO DE PERMANENCIA OCCITESOROS</t>
-  </si>
-  <si>
-    <t>ITAÚ FIDUCIARIA</t>
   </si>
   <si>
     <t>FONDO DE INVERSION COLECTIVA ABIERTO ITAU MONEY MARKET</t>
@@ -144,19 +123,10 @@
     <t>FONDO DE INVERSION COLECTIVA ACCIVAL VISTA</t>
   </si>
   <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO FONDO BBVA DIGITAL</t>
-  </si>
-  <si>
     <t>BTG PACTUAL S.A.</t>
   </si>
   <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA DEL MERCADO MONETARIO BTG PACTUAL LIQUIDEZ</t>
-  </si>
-  <si>
     <t>FONDO DE INVERSION COLECTIVA ABIERTO CONFIRENTA</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO FIDUCUENTA</t>
   </si>
   <si>
     <t>FIDUCIARIA COLMENA S.A.</t>
@@ -174,12 +144,6 @@
     <t>FIDUCOOMEVA</t>
   </si>
   <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO FIC AVANZAR VISTA</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO SIN PACTO DE PERMANENCIA OCCIRENTA</t>
-  </si>
-  <si>
     <t>GLOBAL SECURITIES S.A. COMISIONISTA</t>
   </si>
   <si>
@@ -187,9 +151,6 @@
   </si>
   <si>
     <t>OLD MUTUAL SOCIEDAD FIDUCIARIA S.A.</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA SKANDIA EFECTIVO</t>
   </si>
   <si>
     <t>CARTERA COLECTIVA ABIERTA EFECTIVO A LA VISTA</t>
@@ -204,12 +165,6 @@
     <t>ACCIVAL RENTA FIJA 180</t>
   </si>
   <si>
-    <t>FONDO ABIERTO ALIANZA - SIN PACTO DE PERMANENCIA MÍNIMA</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO CON PACTO DE PERMANENCIA Y  PARTICIPACIONES DIFERENCIALES BBVA</t>
-  </si>
-  <si>
     <t xml:space="preserve">FONDO DE INVERSION COLECTIVA ABIERTO CON PACTO PERMANENCIA ALIANZA RENTA FIJA 90 </t>
   </si>
   <si>
@@ -222,19 +177,10 @@
     <t>FIC MULTIESCALA</t>
   </si>
   <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO FONDO BBVA PÁRAMO</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA RENTA FIJA LARGO PLAZO</t>
-  </si>
-  <si>
     <t>CREDICORP CAPITAL</t>
   </si>
   <si>
     <t>CREDICORP CAPITAL RENTA FIJA COLOMBIA</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO CON PACTO DE PERMANENCIA RENTAPAIS</t>
   </si>
   <si>
     <t>FONDO ABIERTO FIDUCIARIA CENTRAL</t>
@@ -246,12 +192,6 @@
     <t>FONDO DE INVERSION COLECTIVA ABIERTO CON PACTO DE PERMANENCIA PLAN SEMILLA</t>
   </si>
   <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO RENTA FIJA PLAZO</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO CON PACTO DE PERMANENCIA ÓPTIMO</t>
-  </si>
-  <si>
     <t>F.I.C. CON PACTO DE PERMANENCIA CAPITAL PLUS</t>
   </si>
   <si>
@@ -261,12 +201,6 @@
     <t>FONDO DE INVERSION COLECTIVA ABIERTO RENTAR 30</t>
   </si>
   <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO RENTAR</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA FIDUCOLDEX 60 MODERADO,</t>
-  </si>
-  <si>
     <t>FONDO DE INVERSION COLECTIVA ABIERTO CON PACTO DE PERMANENCIA RENTA FIJA DINAMICA</t>
   </si>
   <si>
@@ -274,9 +208,6 @@
   </si>
   <si>
     <t>FONDO DE INVERSION COLECTIVA ABIERTO ITAU CORTO PLAZO</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA SKANDIA MULTIPLAZO</t>
   </si>
   <si>
     <t>CARTERA COLECTIVA ABIERTA CON PACTO DE PERMANENCIA EFECTIVO A PLAZOS - CARTERA CON COMPARTIMENTOS</t>
@@ -291,13 +222,7 @@
     <t xml:space="preserve">FONDO DE INVERSION COLECTIVA ABIERTO CON PACTO DE PERMANENCIA ALIANZA ACCIONES </t>
   </si>
   <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO BTG PACTUAL ACCIONES COLOMBIA</t>
-  </si>
-  <si>
     <t>CREDICORP CAPITAL ACCIONES COLOMBIA</t>
-  </si>
-  <si>
-    <t>FONDO DE INVERSIÓN COLECTIVA ABIERTO RENTA ACCIONES</t>
   </si>
   <si>
     <t>F.I.C. ACCIONES PLUS</t>
@@ -324,9 +249,6 @@
     <t>ACCIONES COLOMBIA PESOS</t>
   </si>
   <si>
-    <t>SKANDIA PENSIONES Y CESANTÍAS S.A.</t>
-  </si>
-  <si>
     <t>PORTAFOLIO SKANDIA STRATEGIST ACCIONES COLOMBIA</t>
   </si>
   <si>
@@ -337,15 +259,6 @@
   </si>
   <si>
     <t xml:space="preserve"> # Inversionistas </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comisión </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Duración </t>
-  </si>
-  <si>
-    <t>Tipo de participación (TP)</t>
   </si>
   <si>
     <t>RN.mensual</t>
@@ -406,6 +319,93 @@
   </si>
   <si>
     <t xml:space="preserve">Valor fondo </t>
+  </si>
+  <si>
+    <t>SKANDIA PENSIONES Y CESANTIAS S.A.</t>
+  </si>
+  <si>
+    <t>FONDO ABIERTO ALIANZA - SIN PACTO DE PERMANENCIA MINIMA</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO BBVA PAIS CON PARTICIPACIONES DIFERENCIALES</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO FIDUCREDICORP VISTA</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTA SIN PACTO DE PERMANENCIA FIDUEXCEDENTES</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO FIDULIQUIDEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FONDO DE INVERSION COLECTIVA FIDUCOLDEX </t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO SIN PACTO DE PERMANENCIA OCCITESOROS</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO FONDO BBVA DIGITAL</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA DEL MERCADO MONETARIO BTG PACTUAL LIQUIDEZ</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO FIDUCUENTA</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO FIC AVANZAR VISTA</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO SIN PACTO DE PERMANENCIA OCCIRENTA</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA SKANDIA EFECTIVO</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO CON PACTO DE PERMANENCIA Y  PARTICIPACIONES DIFERENCIALES BBVA</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO FONDO BBVA PARAMO</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA RENTA FIJA LARGO PLAZO</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO CON PACTO DE PERMANENCIA RENTAPAIS</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO RENTA FIJA PLAZO</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO CON PACTO DE PERMANENCIA OPTIMO</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO RENTAR</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA FIDUCOLDEX 60 MODERADO,</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA SKANDIA MULTIPLAZO</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO BTG PACTUAL ACCIONES COLOMBIA</t>
+  </si>
+  <si>
+    <t>FONDO DE INVERSION COLECTIVA ABIERTO RENTA ACCIONES</t>
+  </si>
+  <si>
+    <t>ITAU FIDUCIARIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comision</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Duracion </t>
+  </si>
+  <si>
+    <t>Tipo de participacion (TP)</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0829DF-FC64-460D-9CD1-CD1ABAEB3F20}">
   <dimension ref="A1:Z281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1020,82 +1020,82 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" t="s">
         <v>122</v>
       </c>
-      <c r="D1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" t="s">
-        <v>102</v>
-      </c>
       <c r="H1" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="J1" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="K1" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="L1" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="M1" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="N1" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="O1" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="P1" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="Q1" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="R1" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="S1" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="T1" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="U1" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="V1" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="W1" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="X1" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="Y1" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="Z1" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
@@ -2019,7 +2019,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="C14" s="3">
         <v>1441712488249.1899</v>
@@ -2099,7 +2099,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="C15" s="3">
         <v>7231455211.4200001</v>
@@ -2175,7 +2175,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="C16" s="3">
         <v>102642017875.84</v>
@@ -2251,7 +2251,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="C17" s="3">
         <v>208995476430.20001</v>
@@ -2324,10 +2324,10 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C18" s="3">
         <v>34015482593.720001</v>
@@ -2400,10 +2400,10 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C19" s="3">
         <v>153736499837.32999</v>
@@ -2476,10 +2476,10 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C20" s="3">
         <v>28335837623.57</v>
@@ -2552,10 +2552,10 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C21" s="3">
         <v>97152013805.970001</v>
@@ -2628,10 +2628,10 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C22" s="3">
         <v>8107634489.3100004</v>
@@ -2704,10 +2704,10 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C23" s="3">
         <v>132522680615.91</v>
@@ -2780,10 +2780,10 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C24" s="3">
         <v>81595684357.220001</v>
@@ -2856,10 +2856,10 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C25" s="3">
         <v>1190818.04</v>
@@ -2932,10 +2932,10 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C26" s="3">
         <v>2950241670.6100001</v>
@@ -3008,10 +3008,10 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C27" s="3">
         <v>269626923754.25</v>
@@ -3088,10 +3088,10 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C28" s="3">
         <v>412846094608.71997</v>
@@ -3164,10 +3164,10 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C29" s="3">
         <v>8581645201.2799997</v>
@@ -3240,10 +3240,10 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="C30" s="3">
         <v>187605386856.79001</v>
@@ -3316,10 +3316,10 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C31" s="3">
         <v>66522703456.720001</v>
@@ -3392,10 +3392,10 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C32" s="3">
         <v>10170248476.51</v>
@@ -3472,10 +3472,10 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C33" s="3">
         <v>13965809561.17</v>
@@ -3548,10 +3548,10 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C34" s="3">
         <v>111697433321.06</v>
@@ -3624,10 +3624,10 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C35" s="3">
         <v>337800234354.47998</v>
@@ -3700,10 +3700,10 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C36" s="3">
         <v>74721510517.860001</v>
@@ -3776,10 +3776,10 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C37" s="3">
         <v>385399204686.60999</v>
@@ -3852,10 +3852,10 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C38" s="3">
         <v>174954871.71000001</v>
@@ -3928,10 +3928,10 @@
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C39" s="3">
         <v>64565178814.559998</v>
@@ -4004,10 +4004,10 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C40" s="3">
         <v>752538749.16999996</v>
@@ -4080,10 +4080,10 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C41" s="3">
         <v>2348627162.2199998</v>
@@ -4156,10 +4156,10 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C42" s="3">
         <v>24548511412.27</v>
@@ -4232,10 +4232,10 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C43" s="3">
         <v>97482800986.990005</v>
@@ -4308,10 +4308,10 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C44" s="3">
         <v>230704857.22</v>
@@ -4384,10 +4384,10 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C45" s="3">
         <v>0</v>
@@ -4460,10 +4460,10 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C46" s="3">
         <v>34695593258.510002</v>
@@ -4536,10 +4536,10 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C47" s="3">
         <v>13893395402.83</v>
@@ -4612,10 +4612,10 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C48" s="3">
         <v>27946299808.290001</v>
@@ -4692,10 +4692,10 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C49" s="3">
         <v>268340309.28999999</v>
@@ -4768,10 +4768,10 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C50" s="3">
         <v>3678433253.0599999</v>
@@ -4844,10 +4844,10 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C51" s="3">
         <v>9535691367.1499996</v>
@@ -4920,10 +4920,10 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C52" s="3">
         <v>12727449490.82</v>
@@ -4996,10 +4996,10 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="C53" s="3">
         <v>1462622937802.76</v>
@@ -5076,10 +5076,10 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C54" s="3">
         <v>11460133774.469999</v>
@@ -5156,10 +5156,10 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C55" s="3">
         <v>143400024939.82999</v>
@@ -5232,10 +5232,10 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C56" s="3">
         <v>568517703278.46997</v>
@@ -5308,10 +5308,10 @@
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C57" s="3">
         <v>166784455207.78</v>
@@ -5384,10 +5384,10 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C58" s="3">
         <v>277524371503.28003</v>
@@ -5460,10 +5460,10 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C59" s="3">
         <v>394935338219.23999</v>
@@ -5536,10 +5536,10 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C60" s="3">
         <v>1644918431309.71</v>
@@ -5612,10 +5612,10 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C61" s="3">
         <v>241536901383.81</v>
@@ -5688,10 +5688,10 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C62" s="3">
         <v>116233471566.67999</v>
@@ -5764,10 +5764,10 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C63" s="3">
         <v>686525023989.43994</v>
@@ -5844,10 +5844,10 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C64" s="3">
         <v>1028705751812.5</v>
@@ -5924,10 +5924,10 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C65" s="3">
         <v>831562167305.47998</v>
@@ -6004,10 +6004,10 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C66" s="3">
         <v>54607295769.620003</v>
@@ -6080,10 +6080,10 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C67" s="3">
         <v>12737436504.700001</v>
@@ -6156,10 +6156,10 @@
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C68" s="3">
         <v>0</v>
@@ -6232,10 +6232,10 @@
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C69" s="3">
         <v>182299149.44999999</v>
@@ -6308,10 +6308,10 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="C70" s="3">
         <v>6612625061.3400002</v>
@@ -6384,10 +6384,10 @@
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="C71" s="3">
         <v>94047013954.389999</v>
@@ -6464,10 +6464,10 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="C72" s="3">
         <v>333964060289.53003</v>
@@ -6540,10 +6540,10 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="C73" s="3">
         <v>46913148242.5</v>
@@ -6616,10 +6616,10 @@
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="C74" s="3">
         <v>93268536024.899994</v>
@@ -6692,10 +6692,10 @@
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="C75" s="3">
         <v>1609673063.0699999</v>
@@ -6768,10 +6768,10 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C76" s="3">
         <v>94389192027.419998</v>
@@ -6844,10 +6844,10 @@
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C77" s="3">
         <v>35160771471.339996</v>
@@ -6920,10 +6920,10 @@
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C78" s="3">
         <v>4927019850.4399996</v>
@@ -7000,10 +7000,10 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C79" s="3">
         <v>106515573</v>
@@ -7076,10 +7076,10 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C80" s="3">
         <v>609325656.87</v>
@@ -7152,10 +7152,10 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C81" s="3">
         <v>65606371846.849998</v>
@@ -7228,10 +7228,10 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C82" s="3">
         <v>88208720727.089996</v>
@@ -7304,10 +7304,10 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C83" s="3">
         <v>15239699628.26</v>
@@ -7380,10 +7380,10 @@
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C84" s="3">
         <v>69513455086.550003</v>
@@ -7460,10 +7460,10 @@
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C85" s="3">
         <v>254869438488.01999</v>
@@ -7536,10 +7536,10 @@
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C86" s="3">
         <v>135778834867.96001</v>
@@ -7612,10 +7612,10 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C87" s="3">
         <v>1160269893308.72</v>
@@ -7688,10 +7688,10 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C88" s="3">
         <v>7616597797.1700001</v>
@@ -7764,10 +7764,10 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C89" s="3">
         <v>6018937602.9799995</v>
@@ -7840,10 +7840,10 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C90" s="3">
         <v>215043432112.87</v>
@@ -7916,10 +7916,10 @@
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C91" s="3">
         <v>33370628247.52</v>
@@ -7992,10 +7992,10 @@
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C92" s="3">
         <v>10033041005.559999</v>
@@ -8068,10 +8068,10 @@
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="C93" s="3">
         <v>11009696522.1</v>
@@ -8144,10 +8144,10 @@
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C94" s="3">
         <v>118672705723.71001</v>
@@ -8220,10 +8220,10 @@
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C95" s="3">
         <v>127656257100.92999</v>
@@ -8296,10 +8296,10 @@
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C96" s="3">
         <v>175736889881.57001</v>
@@ -8372,10 +8372,10 @@
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C97" s="3">
         <v>178500954664.17001</v>
@@ -8452,10 +8452,10 @@
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C98" s="3">
         <v>328419259425.47998</v>
@@ -8528,10 +8528,10 @@
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C99" s="3">
         <v>2840959941413.2002</v>
@@ -8608,10 +8608,10 @@
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C100" s="3">
         <v>57868304575.209999</v>
@@ -8684,10 +8684,10 @@
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C101" s="3">
         <v>105277612078.52</v>
@@ -8760,10 +8760,10 @@
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C102" s="3">
         <v>0</v>
@@ -8836,10 +8836,10 @@
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C103" s="3">
         <v>247585.47</v>
@@ -8912,10 +8912,10 @@
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C104" s="3">
         <v>316521649934.42999</v>
@@ -8995,7 +8995,7 @@
         <v>5</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="C105" s="3">
         <v>170640684571.37</v>
@@ -9072,10 +9072,10 @@
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="C106" s="3">
         <v>409625906003.78998</v>
@@ -9152,10 +9152,10 @@
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="C107" s="3">
         <v>329301720971.52002</v>
@@ -9228,10 +9228,10 @@
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="C108" s="3">
         <v>844193489289.56006</v>
@@ -9304,10 +9304,10 @@
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="C109" s="3">
         <v>155753472896.69</v>
@@ -9380,10 +9380,10 @@
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="C110" s="3">
         <v>44607630671.400002</v>
@@ -9456,10 +9456,10 @@
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="C111" s="3">
         <v>104673086.39</v>
@@ -9532,10 +9532,10 @@
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C112" s="3">
         <v>678630041.89999998</v>
@@ -9608,10 +9608,10 @@
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C113" s="3">
         <v>3654075895.6700001</v>
@@ -9688,10 +9688,10 @@
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C114" s="3">
         <v>335613408.97000003</v>
@@ -9764,10 +9764,10 @@
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C115" s="3">
         <v>85818090.810000002</v>
@@ -9840,10 +9840,10 @@
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C116" s="3">
         <v>10219980991.15</v>
@@ -9916,10 +9916,10 @@
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="C117" s="3">
         <v>13200059582569</v>
@@ -9996,10 +9996,10 @@
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C118" s="3">
         <v>44820999250.150002</v>
@@ -10072,10 +10072,10 @@
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C119" s="3">
         <v>20208511503.299999</v>
@@ -10148,10 +10148,10 @@
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C120" s="3">
         <v>13200271755.76</v>
@@ -10224,10 +10224,10 @@
     </row>
     <row r="121" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C121" s="3">
         <v>1357460774.01</v>
@@ -10300,10 +10300,10 @@
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C122" s="3">
         <v>75622143438.550003</v>
@@ -10376,10 +10376,10 @@
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C123" s="3">
         <v>65790568029.699997</v>
@@ -10452,10 +10452,10 @@
     </row>
     <row r="124" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C124" s="3">
         <v>608736648623.20996</v>
@@ -10532,10 +10532,10 @@
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C125" s="3">
         <v>359483843733.15002</v>
@@ -10612,10 +10612,10 @@
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C126" s="3">
         <v>948057948890.76001</v>
@@ -10692,10 +10692,10 @@
     </row>
     <row r="127" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C127" s="3">
         <v>1018714086549.83</v>
@@ -10768,10 +10768,10 @@
     </row>
     <row r="128" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C128" s="3">
         <v>256705139531.54999</v>
@@ -10844,10 +10844,10 @@
     </row>
     <row r="129" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C129" s="3">
         <v>1717935125571.02</v>
@@ -10920,10 +10920,10 @@
     </row>
     <row r="130" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C130" s="3">
         <v>145607101285.82001</v>
@@ -10996,10 +10996,10 @@
     </row>
     <row r="131" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C131" s="3">
         <v>57607793097.150002</v>
@@ -11072,10 +11072,10 @@
     </row>
     <row r="132" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C132" s="3">
         <v>76684157071.470001</v>
@@ -11148,10 +11148,10 @@
     </row>
     <row r="133" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C133" s="3">
         <v>134567439394.60001</v>
@@ -11224,10 +11224,10 @@
     </row>
     <row r="134" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C134" s="3">
         <v>15019270473.84</v>
@@ -11304,10 +11304,10 @@
     </row>
     <row r="135" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C135" s="3">
         <v>15389252651.129999</v>
@@ -11380,10 +11380,10 @@
     </row>
     <row r="136" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C136" s="3">
         <v>568860227.30999994</v>
@@ -11456,10 +11456,10 @@
     </row>
     <row r="137" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C137" s="3">
         <v>12157018629.5</v>
@@ -11532,10 +11532,10 @@
     </row>
     <row r="138" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C138" s="3">
         <v>38014128455.870003</v>
@@ -11608,10 +11608,10 @@
     </row>
     <row r="139" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C139" s="3">
         <v>8484914033.4899998</v>
@@ -11684,10 +11684,10 @@
     </row>
     <row r="140" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C140" s="3">
         <v>15929657968.32</v>
@@ -11760,10 +11760,10 @@
     </row>
     <row r="141" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C141" s="3">
         <v>2212383764.52</v>
@@ -11836,10 +11836,10 @@
     </row>
     <row r="142" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="C142" s="3">
         <v>327566796201.09003</v>
@@ -11912,10 +11912,10 @@
     </row>
     <row r="143" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="C143" s="3">
         <v>313192335002.87</v>
@@ -11988,10 +11988,10 @@
     </row>
     <row r="144" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="C144" s="3">
         <v>201494306535.10999</v>
@@ -12064,10 +12064,10 @@
     </row>
     <row r="145" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="C145" s="3">
         <v>564816174059.39001</v>
@@ -12144,10 +12144,10 @@
     </row>
     <row r="146" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="C146" s="3">
         <v>916662578997.58997</v>
@@ -12220,10 +12220,10 @@
     </row>
     <row r="147" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C147" s="3">
         <v>40489374867.230003</v>
@@ -12300,10 +12300,10 @@
     </row>
     <row r="148" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C148" s="3">
         <v>110085794717.37</v>
@@ -12376,10 +12376,10 @@
     </row>
     <row r="149" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C149" s="3">
         <v>124132359145.97</v>
@@ -12452,10 +12452,10 @@
     </row>
     <row r="150" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C150" s="3">
         <v>225286846635.12</v>
@@ -12532,10 +12532,10 @@
     </row>
     <row r="151" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C151" s="3">
         <v>115783409082.33</v>
@@ -12608,10 +12608,10 @@
     </row>
     <row r="152" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C152" s="3">
         <v>1366900233.04</v>
@@ -12684,10 +12684,10 @@
     </row>
     <row r="153" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C153" s="3">
         <v>228377.37</v>
@@ -12760,10 +12760,10 @@
     </row>
     <row r="154" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C154" s="3">
         <v>10265169.33</v>
@@ -12836,10 +12836,10 @@
     </row>
     <row r="155" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C155" s="3">
         <v>164179952.77000001</v>
@@ -12912,10 +12912,10 @@
     </row>
     <row r="156" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C156" s="3">
         <v>27832150359.900002</v>
@@ -12988,10 +12988,10 @@
     </row>
     <row r="157" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C157" s="3">
         <v>160105779952.23001</v>
@@ -13064,10 +13064,10 @@
     </row>
     <row r="158" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C158" s="3">
         <v>4599314511.3000002</v>
@@ -13140,10 +13140,10 @@
     </row>
     <row r="159" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C159" s="3">
         <v>7693621583.4099998</v>
@@ -13216,10 +13216,10 @@
     </row>
     <row r="160" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C160" s="3">
         <v>901746752096.57996</v>
@@ -13292,10 +13292,10 @@
     </row>
     <row r="161" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C161" s="3">
         <v>46458078547.059998</v>
@@ -13368,10 +13368,10 @@
     </row>
     <row r="162" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C162" s="3">
         <v>17254843770.880001</v>
@@ -13448,10 +13448,10 @@
     </row>
     <row r="163" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C163" s="3">
         <v>65500078815.510002</v>
@@ -13524,10 +13524,10 @@
     </row>
     <row r="164" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C164" s="3">
         <v>3469169589767.3501</v>
@@ -13604,10 +13604,10 @@
     </row>
     <row r="165" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C165" s="3">
         <v>211297279849.44</v>
@@ -13680,10 +13680,10 @@
     </row>
     <row r="166" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C166" s="3">
         <v>145300377417.51999</v>
@@ -13756,10 +13756,10 @@
     </row>
     <row r="167" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C167" s="3">
         <v>0</v>
@@ -13832,10 +13832,10 @@
     </row>
     <row r="168" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C168" s="3">
         <v>0</v>
@@ -13908,10 +13908,10 @@
     </row>
     <row r="169" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C169" s="3">
         <v>27597263477.16</v>
@@ -13991,7 +13991,7 @@
         <v>0</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C170" s="3">
         <v>1308486211870.77</v>
@@ -14071,7 +14071,7 @@
         <v>0</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C171" s="3">
         <v>308917845590.03003</v>
@@ -14147,7 +14147,7 @@
         <v>0</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C172" s="3">
         <v>2349177.7000000002</v>
@@ -14223,7 +14223,7 @@
         <v>0</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C173" s="3">
         <v>153926562155.14001</v>
@@ -14299,7 +14299,7 @@
         <v>0</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C174" s="3">
         <v>21623031559.939999</v>
@@ -14375,7 +14375,7 @@
         <v>0</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C175" s="3">
         <v>1087761438732.51</v>
@@ -14451,7 +14451,7 @@
         <v>0</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C176" s="3">
         <v>784913630786.08997</v>
@@ -14527,7 +14527,7 @@
         <v>0</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C177" s="3">
         <v>1206163099282.6699</v>
@@ -14603,7 +14603,7 @@
         <v>5</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="C178" s="3">
         <v>102905403313.03999</v>
@@ -14683,7 +14683,7 @@
         <v>0</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C179" s="3">
         <v>611752058368.33997</v>
@@ -14759,7 +14759,7 @@
         <v>0</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C180" s="3">
         <v>279069853988.63</v>
@@ -14835,7 +14835,7 @@
         <v>0</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C181" s="3">
         <v>210262341282.69</v>
@@ -14911,7 +14911,7 @@
         <v>0</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C182" s="3">
         <v>168816532575.04999</v>
@@ -14987,7 +14987,7 @@
         <v>0</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C183" s="3">
         <v>31634127001.52</v>
@@ -15063,7 +15063,7 @@
         <v>0</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C184" s="3">
         <v>15635094954.92</v>
@@ -15143,7 +15143,7 @@
         <v>0</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C185" s="3">
         <v>30067503735.25</v>
@@ -15216,10 +15216,10 @@
     </row>
     <row r="186" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C186" s="3">
         <v>75859155646.490005</v>
@@ -15299,7 +15299,7 @@
         <v>0</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C187" s="3">
         <v>36456578808.370003</v>
@@ -15372,10 +15372,10 @@
     </row>
     <row r="188" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C188" s="3">
         <v>198345715743.12</v>
@@ -15455,7 +15455,7 @@
         <v>0</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C189" s="3">
         <v>68010965518.699997</v>
@@ -15531,7 +15531,7 @@
         <v>0</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C190" s="3">
         <v>59854059699.209999</v>
@@ -15607,7 +15607,7 @@
         <v>0</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C191" s="3">
         <v>19768892892.669998</v>
@@ -15683,7 +15683,7 @@
         <v>0</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C192" s="3">
         <v>720160274.57000005</v>
@@ -15759,7 +15759,7 @@
         <v>0</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C193" s="3">
         <v>16727513271.27</v>
@@ -15835,7 +15835,7 @@
         <v>5</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="C194" s="3">
         <v>17021541231.4</v>
@@ -15915,7 +15915,7 @@
         <v>0</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C195" s="3">
         <v>63615958091.919998</v>
@@ -15988,10 +15988,10 @@
     </row>
     <row r="196" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="C196" s="3">
         <v>83703666505.649994</v>
@@ -16071,7 +16071,7 @@
         <v>5</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="C197" s="3">
         <v>0</v>
@@ -16144,10 +16144,10 @@
     </row>
     <row r="198" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C198" s="3">
         <v>95420646742.389999</v>
@@ -16220,10 +16220,10 @@
     </row>
     <row r="199" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C199" s="3">
         <v>83085883684.789993</v>
@@ -16296,10 +16296,10 @@
     </row>
     <row r="200" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C200" s="3">
         <v>165741069058.16</v>
@@ -16372,10 +16372,10 @@
     </row>
     <row r="201" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C201" s="3">
         <v>54836744176.080002</v>
@@ -16448,10 +16448,10 @@
     </row>
     <row r="202" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C202" s="3">
         <v>1756573564.3900001</v>
@@ -16524,10 +16524,10 @@
     </row>
     <row r="203" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C203" s="3">
         <v>129395954867.16</v>
@@ -16604,10 +16604,10 @@
     </row>
     <row r="204" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C204" s="3">
         <v>12375100744.5</v>
@@ -16680,10 +16680,10 @@
     </row>
     <row r="205" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="C205" s="3">
         <v>5895938857.9499998</v>
@@ -16760,10 +16760,10 @@
     </row>
     <row r="206" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C206" s="3">
         <v>24316953.440000001</v>
@@ -16836,10 +16836,10 @@
     </row>
     <row r="207" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C207" s="3">
         <v>5786111972.7299995</v>
@@ -16912,10 +16912,10 @@
     </row>
     <row r="208" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C208" s="3">
         <v>23014015656.73</v>
@@ -16988,10 +16988,10 @@
     </row>
     <row r="209" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C209" s="3">
         <v>3731338068.9899998</v>
@@ -17064,10 +17064,10 @@
     </row>
     <row r="210" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C210" s="3">
         <v>11007504935.129999</v>
@@ -17140,10 +17140,10 @@
     </row>
     <row r="211" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C211" s="3">
         <v>60195049284.860001</v>
@@ -17216,10 +17216,10 @@
     </row>
     <row r="212" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C212" s="3">
         <v>170898926673.17001</v>
@@ -17296,10 +17296,10 @@
     </row>
     <row r="213" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C213" s="3">
         <v>960637658563.71997</v>
@@ -17376,10 +17376,10 @@
     </row>
     <row r="214" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C214" s="3">
         <v>24606924817.560001</v>
@@ -17452,10 +17452,10 @@
     </row>
     <row r="215" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C215" s="3">
         <v>78209164550.570007</v>
@@ -17528,10 +17528,10 @@
     </row>
     <row r="216" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C216" s="3">
         <v>22261253020.040001</v>
@@ -17604,10 +17604,10 @@
     </row>
     <row r="217" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C217" s="3">
         <v>6758511058.4300003</v>
@@ -17680,10 +17680,10 @@
     </row>
     <row r="218" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C218" s="3">
         <v>642150775710.01001</v>
@@ -17760,10 +17760,10 @@
     </row>
     <row r="219" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="C219" s="3">
         <v>250947571223.76001</v>
@@ -17840,10 +17840,10 @@
     </row>
     <row r="220" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="C220" s="3">
         <v>4647548387.5799999</v>
@@ -17920,10 +17920,10 @@
     </row>
     <row r="221" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C221" s="3">
         <v>12556034822.809999</v>
@@ -18000,10 +18000,10 @@
     </row>
     <row r="222" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C222" s="3">
         <v>30777664118.459999</v>
@@ -18080,10 +18080,10 @@
     </row>
     <row r="223" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C223" s="3">
         <v>22296469815.75</v>
@@ -18160,10 +18160,10 @@
     </row>
     <row r="224" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C224" s="3">
         <v>28151839466.740002</v>
@@ -18236,10 +18236,10 @@
     </row>
     <row r="225" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C225" s="3">
         <v>46945905536.309998</v>
@@ -18312,10 +18312,10 @@
     </row>
     <row r="226" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C226" s="3">
         <v>734396916.09000003</v>
@@ -18388,10 +18388,10 @@
     </row>
     <row r="227" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C227" s="3">
         <v>2382638483.0999999</v>
@@ -18464,10 +18464,10 @@
     </row>
     <row r="228" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C228" s="3">
         <v>19385242201.189999</v>
@@ -18540,10 +18540,10 @@
     </row>
     <row r="229" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C229" s="3">
         <v>706763947.48000002</v>
@@ -18616,10 +18616,10 @@
     </row>
     <row r="230" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C230" s="3">
         <v>146184484892.32999</v>
@@ -18692,10 +18692,10 @@
     </row>
     <row r="231" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C231" s="3">
         <v>44372123753.370003</v>
@@ -18772,10 +18772,10 @@
     </row>
     <row r="232" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C232" s="3">
         <v>922133580.87</v>
@@ -18848,10 +18848,10 @@
     </row>
     <row r="233" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="C233" s="3">
         <v>19714553415.330002</v>
@@ -18928,10 +18928,10 @@
     </row>
     <row r="234" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C234" s="3">
         <v>31107216820.369999</v>
@@ -19008,10 +19008,10 @@
     </row>
     <row r="235" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C235" s="3">
         <v>38077712152.18</v>
@@ -19084,10 +19084,10 @@
     </row>
     <row r="236" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C236" s="3">
         <v>2000960.44</v>
@@ -19160,10 +19160,10 @@
     </row>
     <row r="237" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C237" s="3">
         <v>2306164569.6500001</v>
@@ -19236,10 +19236,10 @@
     </row>
     <row r="238" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C238" s="3">
         <v>36092325458.18</v>
@@ -19312,10 +19312,10 @@
     </row>
     <row r="239" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C239" s="3">
         <v>38415141.060000002</v>
@@ -19388,10 +19388,10 @@
     </row>
     <row r="240" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C240" s="3">
         <v>92310444535.960007</v>
@@ -19468,10 +19468,10 @@
     </row>
     <row r="241" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C241" s="3">
         <v>103090235192.28999</v>
@@ -19544,10 +19544,10 @@
     </row>
     <row r="242" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C242" s="3">
         <v>5333900.3099999996</v>
@@ -19620,10 +19620,10 @@
     </row>
     <row r="243" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C243" s="3">
         <v>32980965832.610001</v>
@@ -19696,10 +19696,10 @@
     </row>
     <row r="244" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C244" s="3">
         <v>2054987200.6199999</v>
@@ -19772,10 +19772,10 @@
     </row>
     <row r="245" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C245" s="3">
         <v>1092697375.9400001</v>
@@ -19848,10 +19848,10 @@
     </row>
     <row r="246" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C246" s="3">
         <v>1619597726.1500001</v>
@@ -19924,10 +19924,10 @@
     </row>
     <row r="247" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C247" s="3">
         <v>9399232928.0300007</v>
@@ -20004,10 +20004,10 @@
     </row>
     <row r="248" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C248" s="3">
         <v>2239906420.25</v>
@@ -20080,10 +20080,10 @@
     </row>
     <row r="249" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C249" s="3">
         <v>9303364115.6399994</v>
@@ -20156,10 +20156,10 @@
     </row>
     <row r="250" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C250" s="3">
         <v>14632952760.120001</v>
@@ -20232,10 +20232,10 @@
     </row>
     <row r="251" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A251" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C251" s="3">
         <v>4095682688.96</v>
@@ -20308,10 +20308,10 @@
     </row>
     <row r="252" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A252" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C252" s="3">
         <v>199216942.96000001</v>
@@ -20384,10 +20384,10 @@
     </row>
     <row r="253" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A253" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C253" s="3">
         <v>96258509529.389999</v>
@@ -20464,10 +20464,10 @@
     </row>
     <row r="254" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C254" s="3">
         <v>80068168.450000003</v>
@@ -20540,10 +20540,10 @@
     </row>
     <row r="255" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A255" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C255" s="3">
         <v>1579963189.4000001</v>
@@ -20616,10 +20616,10 @@
     </row>
     <row r="256" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C256" s="3">
         <v>1207132818.1099999</v>
@@ -20692,10 +20692,10 @@
     </row>
     <row r="257" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C257" s="3">
         <v>175061226439.79999</v>
@@ -20768,10 +20768,10 @@
     </row>
     <row r="258" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C258" s="3">
         <v>1524052246.9400001</v>
@@ -20844,10 +20844,10 @@
     </row>
     <row r="259" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C259" s="3">
         <v>272175699903.45999</v>
@@ -20924,10 +20924,10 @@
     </row>
     <row r="260" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A260" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C260" s="3">
         <v>4357699833.6000004</v>
@@ -21007,7 +21007,7 @@
         <v>0</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C261" s="3">
         <v>2145340073.76</v>
@@ -21087,7 +21087,7 @@
         <v>0</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C262" s="3">
         <v>1565408817.24</v>
@@ -21160,10 +21160,10 @@
     </row>
     <row r="263" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A263" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="C263" s="3">
         <v>6085204421.0699997</v>
@@ -21243,7 +21243,7 @@
         <v>0</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C264" s="3">
         <v>201458296.63</v>
@@ -21319,7 +21319,7 @@
         <v>0</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C265" s="3">
         <v>1003099446.9</v>
@@ -21395,7 +21395,7 @@
         <v>0</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C266" s="3">
         <v>2447035017.8600001</v>
@@ -21471,7 +21471,7 @@
         <v>0</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C267" s="3">
         <v>3261558753.2199998</v>
@@ -21544,10 +21544,10 @@
     </row>
     <row r="268" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A268" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="C268" s="3">
         <v>4496689520.1499996</v>
@@ -21620,10 +21620,10 @@
     </row>
     <row r="269" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A269" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="C269" s="3">
         <v>587422436.75999999</v>
@@ -21696,10 +21696,10 @@
     </row>
     <row r="270" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A270" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="C270" s="3">
         <v>1849113449.21</v>
@@ -21772,10 +21772,10 @@
     </row>
     <row r="271" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A271" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C271" s="3">
         <v>72946298953.399994</v>
@@ -21852,10 +21852,10 @@
     </row>
     <row r="272" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A272" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C272" s="3">
         <v>4161456623.5799999</v>
@@ -21928,10 +21928,10 @@
     </row>
     <row r="273" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A273" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="C273" s="3">
         <v>35493564709.139999</v>
@@ -22008,10 +22008,10 @@
     </row>
     <row r="274" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A274" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="C274" s="3">
         <v>6456946586.4399996</v>
@@ -22088,10 +22088,10 @@
     </row>
     <row r="275" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A275" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="C275" s="3">
         <v>6727106683.3500004</v>
@@ -22168,10 +22168,10 @@
     </row>
     <row r="276" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A276" s="1" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C276" s="3">
         <v>2377621966.52</v>
@@ -22248,10 +22248,10 @@
     </row>
     <row r="277" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A277" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="C277" s="3">
         <v>45939555909.129997</v>
@@ -22324,10 +22324,10 @@
     </row>
     <row r="278" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A278" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="C278" s="3">
         <v>101388115227.52</v>
@@ -22404,10 +22404,10 @@
     </row>
     <row r="279" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A279" s="1" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C279" s="3">
         <v>14415189.460000001</v>
@@ -22480,10 +22480,10 @@
     </row>
     <row r="280" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A280" s="1" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C280" s="3">
         <v>531556.56999999995</v>
@@ -22560,10 +22560,10 @@
     </row>
     <row r="281" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A281" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B281" s="8" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="C281" s="9">
         <v>40260868.020000003</v>

</xml_diff>